<commit_message>
Revenue Trend - This Month chart added
</commit_message>
<xml_diff>
--- a/data/sample-data.xlsx
+++ b/data/sample-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\roqore\Artisan Coffee Co\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\roqore\artisan-coffee-co\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECB9677-C75F-47EE-A07F-6038F371486A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F513970C-5253-47A5-87A7-F757C8F0566F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="12" xr2:uid="{432A8DC7-3C39-436D-BC34-D70F3C1732F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{432A8DC7-3C39-436D-BC34-D70F3C1732F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="530">
   <si>
     <t>customer_id</t>
   </si>
@@ -3306,7 +3306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B82119-240C-431F-97AB-32BBD90BB9CF}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -4758,8 +4758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAA69F5-94F9-47FF-A74B-63587A3E7F03}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4972,7 +4972,7 @@
         <v>245</v>
       </c>
       <c r="H7">
-        <v>45465</v>
+        <v>45462</v>
       </c>
       <c r="I7" t="s">
         <v>256</v>
@@ -5000,8 +5000,8 @@
       <c r="G8" t="s">
         <v>258</v>
       </c>
-      <c r="H8" t="s">
-        <v>214</v>
+      <c r="H8">
+        <v>45465</v>
       </c>
       <c r="I8" t="s">
         <v>259</v>

</xml_diff>